<commit_message>
allocate all round for all core in PMF
</commit_message>
<xml_diff>
--- a/mrg.xlsx
+++ b/mrg.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawu01\Desktop\md\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2297A1BB-7518-4FF2-8110-AD805288F630}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B664B4D-607C-42F2-9046-455DF4C9C655}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="2" xr2:uid="{39627F01-7337-4F89-8A01-1D6EB359A865}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="4" xr2:uid="{39627F01-7337-4F89-8A01-1D6EB359A865}"/>
   </bookViews>
   <sheets>
     <sheet name="v0" sheetId="1" r:id="rId1"/>
     <sheet name="normal" sheetId="2" r:id="rId2"/>
-    <sheet name="FME c0 opt" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId4"/>
-    <sheet name="FME c1" sheetId="5" r:id="rId5"/>
-    <sheet name="FME c0 round2-4" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId3"/>
+    <sheet name="FME c1" sheetId="5" r:id="rId4"/>
+    <sheet name="FME c1 round0" sheetId="7" r:id="rId5"/>
+    <sheet name="FME c0 round1" sheetId="3" r:id="rId6"/>
+    <sheet name="FME c0 round2-4" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="141">
   <si>
     <t>tile</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -496,6 +497,72 @@
   </si>
   <si>
     <t>PMF_F8_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMF C0 Round 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMF C0 Round 1-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">PMF_F8_0 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMF_M16_1_a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">PMF_M16_1_b </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMF_F16_0</t>
+  </si>
+  <si>
+    <t>PMF_M16_0_c</t>
+  </si>
+  <si>
+    <t>PMF_M32_0_a</t>
+  </si>
+  <si>
+    <t>PMF_M32_0_b</t>
+  </si>
+  <si>
+    <t>PMF_F16_1</t>
+  </si>
+  <si>
+    <t>PMF_M16_1_c</t>
+  </si>
+  <si>
+    <t>PMF_M32_0_c</t>
+  </si>
+  <si>
+    <t>PMF_F32_0</t>
+  </si>
+  <si>
+    <t>PMF_F16_2</t>
+  </si>
+  <si>
+    <t>PMF_M16_2_c</t>
+  </si>
+  <si>
+    <t>PMF_M64_0</t>
+  </si>
+  <si>
+    <t>PMF_M64_1</t>
+  </si>
+  <si>
+    <t>PMF_F16_3</t>
+  </si>
+  <si>
+    <t>PMF_M16_3_c</t>
+  </si>
+  <si>
+    <t>PMF C1 round 0-3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3124,890 +3191,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A37FD03-BF78-46BE-832D-3A5B174965E9}">
-  <dimension ref="A1:AB35"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>2</v>
-      </c>
-      <c r="Q2">
-        <v>8</v>
-      </c>
-      <c r="R2">
-        <v>2</v>
-      </c>
-      <c r="S2">
-        <v>4</v>
-      </c>
-      <c r="U2">
-        <v>4</v>
-      </c>
-      <c r="V2">
-        <v>19</v>
-      </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
-      <c r="Y2">
-        <v>2</v>
-      </c>
-      <c r="Z2">
-        <v>23</v>
-      </c>
-      <c r="AA2">
-        <v>-13</v>
-      </c>
-      <c r="AB2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <f>B5+$P$2</f>
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <f>C5+$Q$2</f>
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <f>D5+$R$2</f>
-        <v>12</v>
-      </c>
-      <c r="F5">
-        <f>E5+$S$2</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6">
-        <f>B5+8</f>
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <f t="shared" ref="C6:C8" si="0">B6+$P$2</f>
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <f t="shared" ref="D6:D8" si="1">C6+$Q$2</f>
-        <v>18</v>
-      </c>
-      <c r="E6">
-        <f t="shared" ref="E6:E8" si="2">D6+$R$2</f>
-        <v>20</v>
-      </c>
-      <c r="F6">
-        <f t="shared" ref="F6:F8" si="3">E6+$S$2</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7">
-        <f>B6+8</f>
-        <v>16</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="3"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8">
-        <f>B7+8</f>
-        <v>24</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="2"/>
-        <v>36</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9">
-        <f>E8</f>
-        <v>36</v>
-      </c>
-      <c r="D9">
-        <f>C9+$U$2</f>
-        <v>40</v>
-      </c>
-      <c r="E9">
-        <f>D9+$V$2</f>
-        <v>59</v>
-      </c>
-      <c r="F9">
-        <f>E9+$W$2</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10">
-        <f>F9</f>
-        <v>60</v>
-      </c>
-      <c r="D10">
-        <f>C10+$H$2</f>
-        <v>61</v>
-      </c>
-      <c r="E10">
-        <f>D10+$I$2</f>
-        <v>62</v>
-      </c>
-      <c r="F10">
-        <f>E10+$J$2</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11">
-        <f>F10</f>
-        <v>63</v>
-      </c>
-      <c r="D11">
-        <f>C11+$L$2</f>
-        <v>64</v>
-      </c>
-      <c r="E11">
-        <f>D11+$M$2</f>
-        <v>65</v>
-      </c>
-      <c r="F11">
-        <f>E11+$N$2</f>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B12">
-        <f>D29-2</f>
-        <v>72</v>
-      </c>
-      <c r="C12">
-        <f>B12+$P$2</f>
-        <v>74</v>
-      </c>
-      <c r="D12">
-        <f>C12+$Q$2</f>
-        <v>82</v>
-      </c>
-      <c r="E12">
-        <f>D12+$R$2</f>
-        <v>84</v>
-      </c>
-      <c r="F12">
-        <f>E12+$S$2</f>
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13">
-        <f>E12</f>
-        <v>84</v>
-      </c>
-      <c r="D13">
-        <f>C13+$U$2</f>
-        <v>88</v>
-      </c>
-      <c r="E13">
-        <f>D13+$V$2</f>
-        <v>107</v>
-      </c>
-      <c r="F13">
-        <f>E13+$W$2</f>
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14">
-        <f>F13</f>
-        <v>108</v>
-      </c>
-      <c r="D14">
-        <f>C14+$H$2</f>
-        <v>109</v>
-      </c>
-      <c r="E14">
-        <f>D14+$I$2</f>
-        <v>110</v>
-      </c>
-      <c r="F14">
-        <f>E14+$J$2</f>
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C15">
-        <f>F14</f>
-        <v>111</v>
-      </c>
-      <c r="D15">
-        <f>C15+$L$2</f>
-        <v>112</v>
-      </c>
-      <c r="E15">
-        <f>D15+$M$2</f>
-        <v>113</v>
-      </c>
-      <c r="F15">
-        <f>E15+$N$2</f>
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>106</v>
-      </c>
-      <c r="B16">
-        <f>D32-2</f>
-        <v>119</v>
-      </c>
-      <c r="C16">
-        <f>B16+$P$2</f>
-        <v>121</v>
-      </c>
-      <c r="D16">
-        <f>C16+$Q$2</f>
-        <v>129</v>
-      </c>
-      <c r="E16">
-        <f>D16+$R$2</f>
-        <v>131</v>
-      </c>
-      <c r="F16">
-        <f>E16+$S$2</f>
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>105</v>
-      </c>
-      <c r="C17">
-        <f>E16</f>
-        <v>131</v>
-      </c>
-      <c r="D17">
-        <f>C17+$U$2</f>
-        <v>135</v>
-      </c>
-      <c r="E17">
-        <f>D17+$V$2</f>
-        <v>154</v>
-      </c>
-      <c r="F17">
-        <f>E17+$W$2</f>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18">
-        <f>F17</f>
-        <v>155</v>
-      </c>
-      <c r="D18">
-        <f>C18+$H$2</f>
-        <v>156</v>
-      </c>
-      <c r="E18">
-        <f>D18+$I$2</f>
-        <v>157</v>
-      </c>
-      <c r="F18">
-        <f>E18+$J$2</f>
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>102</v>
-      </c>
-      <c r="C19">
-        <f>F18</f>
-        <v>158</v>
-      </c>
-      <c r="D19">
-        <f>C19+$L$2</f>
-        <v>159</v>
-      </c>
-      <c r="E19">
-        <f>D19+$M$2</f>
-        <v>160</v>
-      </c>
-      <c r="F19">
-        <f>E19+$N$2</f>
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>111</v>
-      </c>
-      <c r="B20">
-        <f>D35-2</f>
-        <v>166</v>
-      </c>
-      <c r="C20">
-        <f>B20+$P$2</f>
-        <v>168</v>
-      </c>
-      <c r="D20">
-        <f>C20+$Q$2</f>
-        <v>176</v>
-      </c>
-      <c r="E20">
-        <f>D20+$R$2</f>
-        <v>178</v>
-      </c>
-      <c r="F20">
-        <f>E20+$S$2</f>
-        <v>182</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21">
-        <f>E20</f>
-        <v>178</v>
-      </c>
-      <c r="D21">
-        <f>C21+$U$2</f>
-        <v>182</v>
-      </c>
-      <c r="E21">
-        <f>D21+$V$2</f>
-        <v>201</v>
-      </c>
-      <c r="F21">
-        <f>E21+$W$2</f>
-        <v>202</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22">
-        <f>F21</f>
-        <v>202</v>
-      </c>
-      <c r="D22">
-        <f>C22+$H$2</f>
-        <v>203</v>
-      </c>
-      <c r="E22">
-        <f>D22+$I$2</f>
-        <v>204</v>
-      </c>
-      <c r="F22">
-        <f>E22+$J$2</f>
-        <v>205</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23">
-        <f>F22</f>
-        <v>205</v>
-      </c>
-      <c r="D23">
-        <f>C23+$L$2</f>
-        <v>206</v>
-      </c>
-      <c r="E23">
-        <f>D23+$M$2</f>
-        <v>207</v>
-      </c>
-      <c r="F23">
-        <f>E23+$N$2</f>
-        <v>208</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24">
-        <f>F23</f>
-        <v>208</v>
-      </c>
-      <c r="E24">
-        <f>D24+7</f>
-        <v>215</v>
-      </c>
-      <c r="F24">
-        <f>E24+1</f>
-        <v>216</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>112</v>
-      </c>
-      <c r="B25">
-        <f>B8+8</f>
-        <v>32</v>
-      </c>
-      <c r="C25">
-        <f t="shared" ref="C25:C26" si="4">B25+$P$2</f>
-        <v>34</v>
-      </c>
-      <c r="D25">
-        <f t="shared" ref="D25:D26" si="5">C25+$Q$2</f>
-        <v>42</v>
-      </c>
-      <c r="E25">
-        <f t="shared" ref="E25:E26" si="6">D25+$R$2</f>
-        <v>44</v>
-      </c>
-      <c r="F25">
-        <f t="shared" ref="F25:F26" si="7">E25+$S$2</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>103</v>
-      </c>
-      <c r="B26">
-        <f>B25+8</f>
-        <v>40</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="4"/>
-        <v>42</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="5"/>
-        <v>50</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="6"/>
-        <v>52</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="7"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>120</v>
-      </c>
-      <c r="B27">
-        <f>B26+8</f>
-        <v>48</v>
-      </c>
-      <c r="C27">
-        <f>B27+$P$2</f>
-        <v>50</v>
-      </c>
-      <c r="D27">
-        <f>C27+$Q$2</f>
-        <v>58</v>
-      </c>
-      <c r="E27">
-        <f>D27+$R$2</f>
-        <v>60</v>
-      </c>
-      <c r="F27">
-        <f>E27+$S$2</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>118</v>
-      </c>
-      <c r="B28">
-        <f>D27-2</f>
-        <v>56</v>
-      </c>
-      <c r="C28">
-        <f>B28+$P$2</f>
-        <v>58</v>
-      </c>
-      <c r="D28">
-        <f>C28+$Q$2</f>
-        <v>66</v>
-      </c>
-      <c r="E28">
-        <f>D28+$R$2</f>
-        <v>68</v>
-      </c>
-      <c r="F28">
-        <f>E28+$S$2</f>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>110</v>
-      </c>
-      <c r="B29">
-        <f>D28-2</f>
-        <v>64</v>
-      </c>
-      <c r="C29">
-        <f>B29+$P$2</f>
-        <v>66</v>
-      </c>
-      <c r="D29">
-        <f>C29+$Q$2</f>
-        <v>74</v>
-      </c>
-      <c r="E29">
-        <f>D29+$R$2</f>
-        <v>76</v>
-      </c>
-      <c r="F29">
-        <f>E29+$S$2</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>114</v>
-      </c>
-      <c r="B30">
-        <f>B12+8</f>
-        <v>80</v>
-      </c>
-      <c r="C30">
-        <f>B30+$P$2</f>
-        <v>82</v>
-      </c>
-      <c r="D30">
-        <f>C30+$Q$2</f>
-        <v>90</v>
-      </c>
-      <c r="E30">
-        <f>D30+$R$2</f>
-        <v>92</v>
-      </c>
-      <c r="F30">
-        <f>E30+$S$2</f>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>115</v>
-      </c>
-      <c r="B31">
-        <f>B30+8</f>
-        <v>88</v>
-      </c>
-      <c r="C31">
-        <f>B31+$P$2</f>
-        <v>90</v>
-      </c>
-      <c r="D31">
-        <f>C31+$Q$2</f>
-        <v>98</v>
-      </c>
-      <c r="E31">
-        <f>D31+$R$2</f>
-        <v>100</v>
-      </c>
-      <c r="F31">
-        <f>E31+$S$2</f>
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>104</v>
-      </c>
-      <c r="B32">
-        <f>B31+8</f>
-        <v>96</v>
-      </c>
-      <c r="C32">
-        <f>B32+$Y$2</f>
-        <v>98</v>
-      </c>
-      <c r="D32">
-        <f>C32+$Z$2</f>
-        <v>121</v>
-      </c>
-      <c r="E32">
-        <f>D32+$AA$2</f>
-        <v>108</v>
-      </c>
-      <c r="F32">
-        <f>E32+$AB$2</f>
-        <v>124</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>109</v>
-      </c>
-      <c r="B33">
-        <f>D16-2</f>
-        <v>127</v>
-      </c>
-      <c r="C33">
-        <f>B33+$Y$2</f>
-        <v>129</v>
-      </c>
-      <c r="D33">
-        <f>C33+$Z$2</f>
-        <v>152</v>
-      </c>
-      <c r="E33">
-        <f>D33+$AA$2</f>
-        <v>139</v>
-      </c>
-      <c r="F33">
-        <f>E33+$AB$2</f>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>107</v>
-      </c>
-      <c r="B34">
-        <f>D33-2</f>
-        <v>150</v>
-      </c>
-      <c r="C34">
-        <f>B34+$P$2</f>
-        <v>152</v>
-      </c>
-      <c r="D34">
-        <f>C34+$Q$2</f>
-        <v>160</v>
-      </c>
-      <c r="E34">
-        <f>D34+$R$2</f>
-        <v>162</v>
-      </c>
-      <c r="F34">
-        <f>E34+$S$2</f>
-        <v>166</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>108</v>
-      </c>
-      <c r="B35">
-        <f>B34+8</f>
-        <v>158</v>
-      </c>
-      <c r="C35">
-        <f>B35+$P$2</f>
-        <v>160</v>
-      </c>
-      <c r="D35">
-        <f>C35+$Q$2</f>
-        <v>168</v>
-      </c>
-      <c r="E35">
-        <f>D35+$R$2</f>
-        <v>170</v>
-      </c>
-      <c r="F35">
-        <f>E35+$S$2</f>
-        <v>174</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DE056F-CC02-4E3B-AB85-0764275BAE41}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4020,12 +3203,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C61D32-D134-4872-8849-727E0AB1D28E}">
   <dimension ref="A1:AB63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H35" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5662,12 +4845,537 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960532D1-4B94-487D-B28D-6E027395071B}">
+  <dimension ref="A1:AB19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K26" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="17" max="17" width="11.125" customWidth="1"/>
+    <col min="18" max="18" width="7.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>78</v>
+      </c>
+      <c r="R2">
+        <v>-25</v>
+      </c>
+      <c r="S2">
+        <v>64</v>
+      </c>
+      <c r="U2">
+        <v>4</v>
+      </c>
+      <c r="V2">
+        <v>19</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>2</v>
+      </c>
+      <c r="Z2">
+        <v>23</v>
+      </c>
+      <c r="AA2">
+        <v>-9</v>
+      </c>
+      <c r="AB2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <f>B5+$Y$2</f>
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <f>C5+$Z$2</f>
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <f>D5+$AA$2</f>
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <f>E5+$AB$2</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ref="B6:B18" si="0">D5-2</f>
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <f>B6+$Y$2</f>
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <f>C6+$Z$2</f>
+        <v>48</v>
+      </c>
+      <c r="E6">
+        <f>D6+$AA$2</f>
+        <v>39</v>
+      </c>
+      <c r="F6">
+        <f>E6+$AB$2</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <f>B7+$P$2</f>
+        <v>48</v>
+      </c>
+      <c r="D7">
+        <f>C7+$Q$2</f>
+        <v>126</v>
+      </c>
+      <c r="E7">
+        <f>D7+$R$2</f>
+        <v>101</v>
+      </c>
+      <c r="F7">
+        <f>E7+$S$2</f>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="C8">
+        <f>B8+$P$2</f>
+        <v>126</v>
+      </c>
+      <c r="D8">
+        <f>C8+$Q$2</f>
+        <v>204</v>
+      </c>
+      <c r="E8">
+        <f>D8+$R$2</f>
+        <v>179</v>
+      </c>
+      <c r="F8">
+        <f>E8+$S$2</f>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>202</v>
+      </c>
+      <c r="C9">
+        <f>B9+$Y$2</f>
+        <v>204</v>
+      </c>
+      <c r="D9">
+        <f>C9+$Z$2</f>
+        <v>227</v>
+      </c>
+      <c r="E9">
+        <f>D9+$AA$2</f>
+        <v>218</v>
+      </c>
+      <c r="F9">
+        <f>E9+$AB$2</f>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+      <c r="C10">
+        <f>B10+$Y$2</f>
+        <v>227</v>
+      </c>
+      <c r="D10">
+        <f>C10+$Z$2</f>
+        <v>250</v>
+      </c>
+      <c r="E10">
+        <f>D10+$AA$2</f>
+        <v>241</v>
+      </c>
+      <c r="F10">
+        <f>E10+$AB$2</f>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>248</v>
+      </c>
+      <c r="C11">
+        <f>B11+$P$2</f>
+        <v>250</v>
+      </c>
+      <c r="D11">
+        <f>C11+$Q$2</f>
+        <v>328</v>
+      </c>
+      <c r="E11">
+        <f>D11+$R$2</f>
+        <v>303</v>
+      </c>
+      <c r="F11">
+        <f>E11+$S$2</f>
+        <v>367</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>326</v>
+      </c>
+      <c r="C12">
+        <f>B12+$P$2</f>
+        <v>328</v>
+      </c>
+      <c r="D12">
+        <f>C12+$Q$2</f>
+        <v>406</v>
+      </c>
+      <c r="E12">
+        <f>D12+$R$2</f>
+        <v>381</v>
+      </c>
+      <c r="F12">
+        <f>E12+$S$2</f>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>404</v>
+      </c>
+      <c r="C13">
+        <f>B13+$Y$2</f>
+        <v>406</v>
+      </c>
+      <c r="D13">
+        <f>C13+$Z$2</f>
+        <v>429</v>
+      </c>
+      <c r="E13">
+        <f>D13+$AA$2</f>
+        <v>420</v>
+      </c>
+      <c r="F13">
+        <f>E13+$AB$2</f>
+        <v>436</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>427</v>
+      </c>
+      <c r="C14">
+        <f>B14+$Y$2</f>
+        <v>429</v>
+      </c>
+      <c r="D14">
+        <f>C14+$Z$2</f>
+        <v>452</v>
+      </c>
+      <c r="E14">
+        <f>D14+$AA$2</f>
+        <v>443</v>
+      </c>
+      <c r="F14">
+        <f>E14+$AB$2</f>
+        <v>459</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+      <c r="C15">
+        <f>B15+$P$2</f>
+        <v>452</v>
+      </c>
+      <c r="D15">
+        <f>C15+$Q$2</f>
+        <v>530</v>
+      </c>
+      <c r="E15">
+        <f>D15+$R$2</f>
+        <v>505</v>
+      </c>
+      <c r="F15">
+        <f>E15+$S$2</f>
+        <v>569</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>528</v>
+      </c>
+      <c r="C16">
+        <f>B16+$P$2</f>
+        <v>530</v>
+      </c>
+      <c r="D16">
+        <f>C16+$Q$2</f>
+        <v>608</v>
+      </c>
+      <c r="E16">
+        <f>D16+$R$2</f>
+        <v>583</v>
+      </c>
+      <c r="F16">
+        <f>E16+$S$2</f>
+        <v>647</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>606</v>
+      </c>
+      <c r="C17">
+        <f>B17+$Y$2</f>
+        <v>608</v>
+      </c>
+      <c r="D17">
+        <f>C17+$Z$2</f>
+        <v>631</v>
+      </c>
+      <c r="E17">
+        <f>D17+$AA$2</f>
+        <v>622</v>
+      </c>
+      <c r="F17">
+        <f>E17+$AB$2</f>
+        <v>638</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" s="2">
+        <f t="shared" si="0"/>
+        <v>629</v>
+      </c>
+      <c r="C18" s="2">
+        <f>B18+$Y$2</f>
+        <v>631</v>
+      </c>
+      <c r="D18" s="2">
+        <f>C18+$Z$2</f>
+        <v>654</v>
+      </c>
+      <c r="E18" s="2">
+        <f>D18+$AA$2</f>
+        <v>645</v>
+      </c>
+      <c r="F18" s="2">
+        <f>E18+$AB$2</f>
+        <v>661</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E5722B-E97D-444F-8BBA-4F33D9EFBAF8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A37FD03-BF78-46BE-832D-3A5B174965E9}">
   <dimension ref="A1:AB35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5681,7 +5389,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>121</v>
       </c>
       <c r="H1" t="s">
         <v>22</v>
@@ -5827,23 +5535,23 @@
         <v>97</v>
       </c>
       <c r="B5">
-        <v>-30</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <f>B5+$P$2</f>
-        <v>-28</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <f>C5+$Q$2</f>
-        <v>-20</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <f>D5+$R$2</f>
-        <v>-18</v>
+        <v>12</v>
       </c>
       <c r="F5">
         <f>E5+$S$2</f>
-        <v>-14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
@@ -5852,48 +5560,933 @@
       </c>
       <c r="B6">
         <f>B5+8</f>
-        <v>-22</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C8" si="0">B6+$P$2</f>
-        <v>-20</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D8" si="1">C6+$Q$2</f>
-        <v>-12</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <f t="shared" ref="E6:E8" si="2">D6+$R$2</f>
-        <v>-10</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:F8" si="3">E6+$S$2</f>
-        <v>-6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="B7">
         <f>B6+8</f>
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8">
+        <f>B7+8</f>
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <f>E8</f>
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <f>C9+$U$2</f>
+        <v>40</v>
+      </c>
+      <c r="E9">
+        <f>D9+$V$2</f>
+        <v>59</v>
+      </c>
+      <c r="F9">
+        <f>E9+$W$2</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10">
+        <f>F9</f>
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <f>C10+$H$2</f>
+        <v>61</v>
+      </c>
+      <c r="E10">
+        <f>D10+$I$2</f>
+        <v>62</v>
+      </c>
+      <c r="F10">
+        <f>E10+$J$2</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11">
+        <f>F10</f>
+        <v>63</v>
+      </c>
+      <c r="D11">
+        <f>C11+$L$2</f>
+        <v>64</v>
+      </c>
+      <c r="E11">
+        <f>D11+$M$2</f>
+        <v>65</v>
+      </c>
+      <c r="F11">
+        <f>E11+$N$2</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12">
+        <f>D29-2</f>
+        <v>72</v>
+      </c>
+      <c r="C12">
+        <f>B12+$P$2</f>
+        <v>74</v>
+      </c>
+      <c r="D12">
+        <f>C12+$Q$2</f>
+        <v>82</v>
+      </c>
+      <c r="E12">
+        <f>D12+$R$2</f>
+        <v>84</v>
+      </c>
+      <c r="F12">
+        <f>E12+$S$2</f>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13">
+        <f>E12</f>
+        <v>84</v>
+      </c>
+      <c r="D13">
+        <f>C13+$U$2</f>
+        <v>88</v>
+      </c>
+      <c r="E13">
+        <f>D13+$V$2</f>
+        <v>107</v>
+      </c>
+      <c r="F13">
+        <f>E13+$W$2</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14">
+        <f>F13</f>
+        <v>108</v>
+      </c>
+      <c r="D14">
+        <f>C14+$H$2</f>
+        <v>109</v>
+      </c>
+      <c r="E14">
+        <f>D14+$I$2</f>
+        <v>110</v>
+      </c>
+      <c r="F14">
+        <f>E14+$J$2</f>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15">
+        <f>F14</f>
+        <v>111</v>
+      </c>
+      <c r="D15">
+        <f>C15+$L$2</f>
+        <v>112</v>
+      </c>
+      <c r="E15">
+        <f>D15+$M$2</f>
+        <v>113</v>
+      </c>
+      <c r="F15">
+        <f>E15+$N$2</f>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16">
+        <f>D32-2</f>
+        <v>119</v>
+      </c>
+      <c r="C16">
+        <f>B16+$P$2</f>
+        <v>121</v>
+      </c>
+      <c r="D16">
+        <f>C16+$Q$2</f>
+        <v>129</v>
+      </c>
+      <c r="E16">
+        <f>D16+$R$2</f>
+        <v>131</v>
+      </c>
+      <c r="F16">
+        <f>E16+$S$2</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17">
+        <f>E16</f>
+        <v>131</v>
+      </c>
+      <c r="D17">
+        <f>C17+$U$2</f>
+        <v>135</v>
+      </c>
+      <c r="E17">
+        <f>D17+$V$2</f>
+        <v>154</v>
+      </c>
+      <c r="F17">
+        <f>E17+$W$2</f>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18">
+        <f>F17</f>
+        <v>155</v>
+      </c>
+      <c r="D18">
+        <f>C18+$H$2</f>
+        <v>156</v>
+      </c>
+      <c r="E18">
+        <f>D18+$I$2</f>
+        <v>157</v>
+      </c>
+      <c r="F18">
+        <f>E18+$J$2</f>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19">
+        <f>F18</f>
+        <v>158</v>
+      </c>
+      <c r="D19">
+        <f>C19+$L$2</f>
+        <v>159</v>
+      </c>
+      <c r="E19">
+        <f>D19+$M$2</f>
+        <v>160</v>
+      </c>
+      <c r="F19">
+        <f>E19+$N$2</f>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20">
+        <f>D35-2</f>
+        <v>166</v>
+      </c>
+      <c r="C20">
+        <f>B20+$P$2</f>
+        <v>168</v>
+      </c>
+      <c r="D20">
+        <f>C20+$Q$2</f>
+        <v>176</v>
+      </c>
+      <c r="E20">
+        <f>D20+$R$2</f>
+        <v>178</v>
+      </c>
+      <c r="F20">
+        <f>E20+$S$2</f>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21">
+        <f>E20</f>
+        <v>178</v>
+      </c>
+      <c r="D21">
+        <f>C21+$U$2</f>
+        <v>182</v>
+      </c>
+      <c r="E21">
+        <f>D21+$V$2</f>
+        <v>201</v>
+      </c>
+      <c r="F21">
+        <f>E21+$W$2</f>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22">
+        <f>F21</f>
+        <v>202</v>
+      </c>
+      <c r="D22">
+        <f>C22+$H$2</f>
+        <v>203</v>
+      </c>
+      <c r="E22">
+        <f>D22+$I$2</f>
+        <v>204</v>
+      </c>
+      <c r="F22">
+        <f>E22+$J$2</f>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23">
+        <f>F22</f>
+        <v>205</v>
+      </c>
+      <c r="D23">
+        <f>C23+$L$2</f>
+        <v>206</v>
+      </c>
+      <c r="E23">
+        <f>D23+$M$2</f>
+        <v>207</v>
+      </c>
+      <c r="F23">
+        <f>E23+$N$2</f>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24">
+        <f>F23</f>
+        <v>208</v>
+      </c>
+      <c r="E24">
+        <f>D24+7</f>
+        <v>215</v>
+      </c>
+      <c r="F24">
+        <f>E24+1</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25">
+        <f>B8+8</f>
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:C26" si="4">B25+$P$2</f>
+        <v>34</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ref="D25:D26" si="5">C25+$Q$2</f>
+        <v>42</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ref="E25:E26" si="6">D25+$R$2</f>
+        <v>44</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ref="F25:F26" si="7">E25+$S$2</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26">
+        <f>B25+8</f>
+        <v>40</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="6"/>
+        <v>52</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="7"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27">
+        <f>B26+8</f>
+        <v>48</v>
+      </c>
+      <c r="C27">
+        <f>B27+$P$2</f>
+        <v>50</v>
+      </c>
+      <c r="D27">
+        <f>C27+$Q$2</f>
+        <v>58</v>
+      </c>
+      <c r="E27">
+        <f>D27+$R$2</f>
+        <v>60</v>
+      </c>
+      <c r="F27">
+        <f>E27+$S$2</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28">
+        <f>D27-2</f>
+        <v>56</v>
+      </c>
+      <c r="C28">
+        <f>B28+$P$2</f>
+        <v>58</v>
+      </c>
+      <c r="D28">
+        <f>C28+$Q$2</f>
+        <v>66</v>
+      </c>
+      <c r="E28">
+        <f>D28+$R$2</f>
+        <v>68</v>
+      </c>
+      <c r="F28">
+        <f>E28+$S$2</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29">
+        <f>D28-2</f>
+        <v>64</v>
+      </c>
+      <c r="C29">
+        <f>B29+$P$2</f>
+        <v>66</v>
+      </c>
+      <c r="D29">
+        <f>C29+$Q$2</f>
+        <v>74</v>
+      </c>
+      <c r="E29">
+        <f>D29+$R$2</f>
+        <v>76</v>
+      </c>
+      <c r="F29">
+        <f>E29+$S$2</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30">
+        <f>B12+8</f>
+        <v>80</v>
+      </c>
+      <c r="C30">
+        <f>B30+$P$2</f>
+        <v>82</v>
+      </c>
+      <c r="D30">
+        <f>C30+$Q$2</f>
+        <v>90</v>
+      </c>
+      <c r="E30">
+        <f>D30+$R$2</f>
+        <v>92</v>
+      </c>
+      <c r="F30">
+        <f>E30+$S$2</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31">
+        <f>B30+8</f>
+        <v>88</v>
+      </c>
+      <c r="C31">
+        <f>B31+$P$2</f>
+        <v>90</v>
+      </c>
+      <c r="D31">
+        <f>C31+$Q$2</f>
+        <v>98</v>
+      </c>
+      <c r="E31">
+        <f>D31+$R$2</f>
+        <v>100</v>
+      </c>
+      <c r="F31">
+        <f>E31+$S$2</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32">
+        <f>B31+8</f>
+        <v>96</v>
+      </c>
+      <c r="C32">
+        <f>B32+$Y$2</f>
+        <v>98</v>
+      </c>
+      <c r="D32">
+        <f>C32+$Z$2</f>
+        <v>121</v>
+      </c>
+      <c r="E32">
+        <f>D32+$AA$2</f>
+        <v>108</v>
+      </c>
+      <c r="F32">
+        <f>E32+$AB$2</f>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33">
+        <f>D16-2</f>
+        <v>127</v>
+      </c>
+      <c r="C33">
+        <f>B33+$Y$2</f>
+        <v>129</v>
+      </c>
+      <c r="D33">
+        <f>C33+$Z$2</f>
+        <v>152</v>
+      </c>
+      <c r="E33">
+        <f>D33+$AA$2</f>
+        <v>139</v>
+      </c>
+      <c r="F33">
+        <f>E33+$AB$2</f>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34">
+        <f>D33-2</f>
+        <v>150</v>
+      </c>
+      <c r="C34">
+        <f>B34+$P$2</f>
+        <v>152</v>
+      </c>
+      <c r="D34">
+        <f>C34+$Q$2</f>
+        <v>160</v>
+      </c>
+      <c r="E34">
+        <f>D34+$R$2</f>
+        <v>162</v>
+      </c>
+      <c r="F34">
+        <f>E34+$S$2</f>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35">
+        <f>B34+8</f>
+        <v>158</v>
+      </c>
+      <c r="C35">
+        <f>B35+$P$2</f>
+        <v>160</v>
+      </c>
+      <c r="D35">
+        <f>C35+$Q$2</f>
+        <v>168</v>
+      </c>
+      <c r="E35">
+        <f>D35+$R$2</f>
+        <v>170</v>
+      </c>
+      <c r="F35">
+        <f>E35+$S$2</f>
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E5722B-E97D-444F-8BBA-4F33D9EFBAF8}">
+  <dimension ref="A1:AB34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>8</v>
+      </c>
+      <c r="R2">
+        <v>2</v>
+      </c>
+      <c r="S2">
+        <v>4</v>
+      </c>
+      <c r="U2">
+        <v>4</v>
+      </c>
+      <c r="V2">
+        <v>19</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>2</v>
+      </c>
+      <c r="Z2">
+        <v>23</v>
+      </c>
+      <c r="AA2">
+        <v>-13</v>
+      </c>
+      <c r="AB2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5">
+        <v>-24</v>
+      </c>
+      <c r="C5">
+        <f>B5+$P$2</f>
+        <v>-22</v>
+      </c>
+      <c r="D5">
+        <f>C5+$Q$2</f>
         <v>-14</v>
+      </c>
+      <c r="E5">
+        <f>D5+$R$2</f>
+        <v>-12</v>
+      </c>
+      <c r="F5">
+        <f>E5+$S$2</f>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6">
+        <f>B5+8</f>
+        <v>-16</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:C8" si="0">B6+$P$2</f>
+        <v>-14</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D8" si="1">C6+$Q$2</f>
+        <v>-6</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E8" si="2">D6+$R$2</f>
+        <v>-4</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F8" si="3">E6+$S$2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7">
+        <f>B6+8</f>
+        <v>-8</v>
       </c>
       <c r="C7">
         <f>B7+$P$2</f>
-        <v>-12</v>
+        <v>-6</v>
       </c>
       <c r="D7">
         <f>C7+$Q$2</f>
-        <v>-4</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <f>D7+$R$2</f>
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="F7">
         <f>E7+$S$2</f>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
@@ -5988,24 +6581,24 @@
         <v>113</v>
       </c>
       <c r="B12">
-        <f>F11</f>
-        <v>42</v>
+        <f>D28-2</f>
+        <v>48</v>
       </c>
       <c r="C12">
         <f>B12+$P$2</f>
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D12">
         <f>C12+$Q$2</f>
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E12">
         <f>D12+$R$2</f>
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F12">
         <f>E12+$S$2</f>
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
@@ -6014,19 +6607,19 @@
       </c>
       <c r="C13">
         <f>E12</f>
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D13">
         <f>C13+$U$2</f>
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E13">
         <f>D13+$V$2</f>
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F13">
         <f>E13+$W$2</f>
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
@@ -6035,19 +6628,19 @@
       </c>
       <c r="C14">
         <f>F13</f>
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D14">
         <f>C14+$H$2</f>
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E14">
         <f>D14+$I$2</f>
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F14">
         <f>E14+$J$2</f>
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
@@ -6056,19 +6649,19 @@
       </c>
       <c r="C15">
         <f>F14</f>
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D15">
         <f>C15+$L$2</f>
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E15">
         <f>D15+$M$2</f>
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F15">
         <f>E15+$N$2</f>
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
@@ -6077,23 +6670,23 @@
       </c>
       <c r="B16">
         <f>D31-2</f>
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C16">
         <f>B16+$P$2</f>
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D16">
         <f>C16+$Q$2</f>
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E16">
         <f>D16+$R$2</f>
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="F16">
         <f>E16+$S$2</f>
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -6102,19 +6695,19 @@
       </c>
       <c r="C17">
         <f>E16</f>
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D17">
         <f>C17+$U$2</f>
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E17">
         <f>D17+$V$2</f>
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="F17">
         <f>E17+$W$2</f>
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -6123,19 +6716,19 @@
       </c>
       <c r="C18">
         <f>F17</f>
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D18">
         <f>C18+$H$2</f>
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E18">
         <f>D18+$I$2</f>
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="F18">
         <f>E18+$J$2</f>
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -6144,19 +6737,19 @@
       </c>
       <c r="C19">
         <f>F18</f>
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D19">
         <f>C19+$L$2</f>
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E19">
         <f>D19+$M$2</f>
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F19">
         <f>E19+$N$2</f>
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -6165,23 +6758,23 @@
       </c>
       <c r="B20">
         <f>D34-2</f>
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="C20">
         <f>B20+$P$2</f>
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="D20">
         <f>C20+$Q$2</f>
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="E20">
         <f>D20+$R$2</f>
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="F20">
         <f>E20+$S$2</f>
-        <v>137</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -6190,19 +6783,19 @@
       </c>
       <c r="C21">
         <f>E20</f>
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="D21">
         <f>C21+$U$2</f>
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="E21">
         <f>D21+$V$2</f>
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="F21">
         <f>E21+$W$2</f>
-        <v>157</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -6211,19 +6804,19 @@
       </c>
       <c r="C22">
         <f>F21</f>
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="D22">
         <f>C22+$H$2</f>
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E22">
         <f>D22+$I$2</f>
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="F22">
         <f>E22+$J$2</f>
-        <v>160</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -6232,136 +6825,144 @@
       </c>
       <c r="C23">
         <f>F22</f>
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="D23">
         <f>C23+$L$2</f>
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="E23">
         <f>D23+$M$2</f>
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="F23">
         <f>E23+$N$2</f>
-        <v>163</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>112</v>
+      </c>
+      <c r="B24">
+        <f>D8-2</f>
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:C25" si="4">B24+$P$2</f>
+        <v>10</v>
       </c>
       <c r="D24">
-        <f>F23</f>
-        <v>163</v>
+        <f t="shared" ref="D24:D25" si="5">C24+$Q$2</f>
+        <v>18</v>
       </c>
       <c r="E24">
-        <f>D24+7</f>
-        <v>170</v>
+        <f t="shared" ref="E24:E25" si="6">D24+$R$2</f>
+        <v>20</v>
       </c>
       <c r="F24">
-        <f>E24+1</f>
-        <v>171</v>
+        <f t="shared" ref="F24:F25" si="7">E24+$S$2</f>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B25">
-        <f>D8-2</f>
-        <v>8</v>
+        <f>B24+8</f>
+        <v>16</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25:C26" si="4">B25+$P$2</f>
-        <v>10</v>
+        <f t="shared" si="4"/>
+        <v>18</v>
       </c>
       <c r="D25">
-        <f t="shared" ref="D25:D26" si="5">C25+$Q$2</f>
-        <v>18</v>
+        <f t="shared" si="5"/>
+        <v>26</v>
       </c>
       <c r="E25">
-        <f t="shared" ref="E25:E26" si="6">D25+$R$2</f>
-        <v>20</v>
+        <f t="shared" si="6"/>
+        <v>28</v>
       </c>
       <c r="F25">
-        <f t="shared" ref="F25:F26" si="7">E25+$S$2</f>
-        <v>24</v>
+        <f t="shared" si="7"/>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="B26">
         <f>B25+8</f>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C26">
-        <f t="shared" si="4"/>
-        <v>18</v>
+        <f>B26+$P$2</f>
+        <v>26</v>
       </c>
       <c r="D26">
-        <f t="shared" si="5"/>
-        <v>26</v>
+        <f>C26+$Q$2</f>
+        <v>34</v>
       </c>
       <c r="E26">
-        <f t="shared" si="6"/>
-        <v>28</v>
+        <f>D26+$R$2</f>
+        <v>36</v>
       </c>
       <c r="F26">
-        <f t="shared" si="7"/>
-        <v>32</v>
+        <f>E26+$S$2</f>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B27">
-        <f>B26+8</f>
-        <v>24</v>
+        <f>D26-2</f>
+        <v>32</v>
       </c>
       <c r="C27">
         <f>B27+$P$2</f>
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D27">
         <f>C27+$Q$2</f>
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E27">
         <f>D27+$R$2</f>
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F27">
         <f>E27+$S$2</f>
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B28">
         <f>D27-2</f>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C28">
         <f>B28+$P$2</f>
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D28">
         <f>C28+$Q$2</f>
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E28">
         <f>D28+$R$2</f>
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="F28">
         <f>E28+$S$2</f>
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -6370,23 +6971,23 @@
       </c>
       <c r="B29">
         <f>B12+8</f>
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C29">
         <f>B29+$P$2</f>
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D29">
         <f>C29+$Q$2</f>
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E29">
         <f>D29+$R$2</f>
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F29">
         <f>E29+$S$2</f>
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -6395,48 +6996,48 @@
       </c>
       <c r="B30">
         <f>B29+8</f>
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C30">
         <f>B30+$P$2</f>
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D30">
         <f>C30+$Q$2</f>
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E30">
         <f>D30+$R$2</f>
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="F30">
         <f>E30+$S$2</f>
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="B31">
         <f>B30+8</f>
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C31">
         <f>B31+$Y$2</f>
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D31">
         <f>C31+$Z$2</f>
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E31">
         <f>D31+$AA$2</f>
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="F31">
         <f>E31+$AB$2</f>
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -6445,23 +7046,23 @@
       </c>
       <c r="B32">
         <f>D16-2</f>
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C32">
         <f>B32+$P$2</f>
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D32">
         <f>C32+$Q$2</f>
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E32">
         <f>D32+$R$2</f>
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="F32">
         <f>E32+$S$2</f>
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -6470,76 +7071,52 @@
       </c>
       <c r="B33">
         <f>B32+8</f>
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C33">
         <f>B33+$P$2</f>
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D33">
         <f>C33+$Q$2</f>
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E33">
         <f>D33+$R$2</f>
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F33">
         <f>E33+$S$2</f>
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="B34">
         <f>D33-2</f>
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C34">
-        <f>B34+$P$2</f>
-        <v>115</v>
+        <f>B34+$Y$2</f>
+        <v>121</v>
       </c>
       <c r="D34">
-        <f>C34+$Q$2</f>
-        <v>123</v>
+        <f>C34+$Z$2</f>
+        <v>144</v>
       </c>
       <c r="E34">
-        <f>D34+$R$2</f>
-        <v>125</v>
+        <f>D34+$AA$2</f>
+        <v>131</v>
       </c>
       <c r="F34">
-        <f>E34+$S$2</f>
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>109</v>
-      </c>
-      <c r="B35">
-        <f>D20-2</f>
-        <v>129</v>
-      </c>
-      <c r="C35">
-        <f>B35+$Y$2</f>
-        <v>131</v>
-      </c>
-      <c r="D35">
-        <f>C35+$Z$2</f>
-        <v>154</v>
-      </c>
-      <c r="E35">
-        <f>D35+$AA$2</f>
-        <v>141</v>
-      </c>
-      <c r="F35">
-        <f>E35+$AB$2</f>
-        <v>157</v>
+        <f>E34+$AB$2</f>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor: standardize PMF task names and optimize size extraction logic
- Updated PMF task identifiers in CSV files to follow consistent naming convention (e.g., PMF_M32_a split into PMF_32M16_0 and PMF_32M16_1)
- Refactored get_size function in process_excel_and_generate_gantts.py to use regex for better maintainability
- Regenerated corresponding PNG plots and summary files to reflect changes
</commit_message>
<xml_diff>
--- a/mrg.xlsx
+++ b/mrg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawu01\Desktop\md\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E658F3A-6AAD-4A1C-9D17-106DF1227100}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55613F48-645F-41B8-967B-25E08133B339}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="5" xr2:uid="{39627F01-7337-4F89-8A01-1D6EB359A865}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{39627F01-7337-4F89-8A01-1D6EB359A865}"/>
   </bookViews>
   <sheets>
     <sheet name="v0" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="213">
   <si>
     <t>tile</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -283,12 +283,6 @@
     <t>PMF_M16_2_c</t>
   </si>
   <si>
-    <t>PMF_M64_0</t>
-  </si>
-  <si>
-    <t>PMF_M64_1</t>
-  </si>
-  <si>
     <t>PMF_F16_3</t>
   </si>
   <si>
@@ -675,10 +669,6 @@
     <t>PMF_M8_2_c</t>
   </si>
   <si>
-    <t>PMF_M32_a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PMF_F8_3</t>
   </si>
   <si>
@@ -698,6 +688,78 @@
   </si>
   <si>
     <t>PMF c1 round0-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMF_64M32_0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMF_64M32_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMF_32M16_0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMF_32M16_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通道4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y8x8 split</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通道8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y8x8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通道16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMF_2_TQITQ 占用时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通道32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y32x32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y64x64(切成4个32x32)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y16x16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">UV16x16 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">UV8x8 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uv4x4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UV32x32（切成4个16x16)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -705,7 +767,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -781,6 +843,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -790,7 +861,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -962,13 +1033,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFDEE0E3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFDEE0E3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFDEE0E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFDEE0E3"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFDEE0E3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFDEE0E3"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFDEE0E3"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFDEE0E3"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1078,6 +1201,45 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1394,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E39466-5853-41C3-ACC8-1F2734C6766C}">
-  <dimension ref="A1:U203"/>
+  <dimension ref="A1:U204"/>
   <sheetViews>
-    <sheetView topLeftCell="C11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1407,19 +1569,19 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="F1" s="2">
         <v>420</v>
@@ -1428,7 +1590,7 @@
         <v>422</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -1446,7 +1608,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2">
         <v>64</v>
@@ -1458,16 +1620,16 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1485,7 +1647,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B3" s="2">
         <v>16</v>
@@ -1497,16 +1659,16 @@
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -1524,7 +1686,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
@@ -1536,16 +1698,16 @@
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -1563,7 +1725,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -1578,13 +1740,13 @@
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -1625,7 +1787,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B7" s="4">
         <v>3200</v>
@@ -1652,7 +1814,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
@@ -1677,68 +1839,68 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M9" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U9" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="P9" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q9" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="R9" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="S9" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="T9" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="U9" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10" s="8">
         <v>64</v>
@@ -1755,10 +1917,10 @@
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I10" s="8">
         <v>64</v>
@@ -1777,10 +1939,10 @@
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="P10" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="Q10" s="8">
         <v>64</v>
@@ -1801,7 +1963,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B11" s="8">
         <v>16</v>
@@ -1819,7 +1981,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="25"/>
       <c r="H11" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I11" s="8">
         <v>16</v>
@@ -1837,7 +1999,7 @@
       <c r="N11" s="3"/>
       <c r="O11" s="26"/>
       <c r="P11" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q11" s="8">
         <v>16</v>
@@ -1856,7 +2018,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B12" s="8">
         <v>4</v>
@@ -1874,7 +2036,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="26"/>
       <c r="H12" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I12" s="7">
         <v>4</v>
@@ -1891,10 +2053,10 @@
       <c r="M12" s="29"/>
       <c r="N12" s="3"/>
       <c r="O12" s="30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Q12" s="8">
         <v>16</v>
@@ -1915,7 +2077,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B13" s="8">
         <v>4</v>
@@ -1932,10 +2094,10 @@
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I13" s="8">
         <v>4</v>
@@ -1955,7 +2117,7 @@
       <c r="N13" s="3"/>
       <c r="O13" s="31"/>
       <c r="P13" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Q13" s="8">
         <v>4</v>
@@ -1983,7 +2145,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="32"/>
       <c r="H14" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I14" s="8">
         <v>4</v>
@@ -2001,7 +2163,7 @@
       <c r="N14" s="3"/>
       <c r="O14" s="32"/>
       <c r="P14" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q14" s="8">
         <v>4</v>
@@ -2043,66 +2205,66 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="4"/>
       <c r="G16" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M16" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="N16" s="3"/>
       <c r="O16" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="P16" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q16" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="R16" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U16" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="P16" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q16" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="R16" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="S16" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="T16" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="U16" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B17" s="8">
         <v>64</v>
@@ -2119,10 +2281,10 @@
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I17" s="8">
         <v>64</v>
@@ -2141,10 +2303,10 @@
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Q17" s="8">
         <v>64</v>
@@ -2165,7 +2327,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="33" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B18" s="8">
         <v>16</v>
@@ -2183,7 +2345,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="25"/>
       <c r="H18" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I18" s="8">
         <v>16</v>
@@ -2201,7 +2363,7 @@
       <c r="N18" s="3"/>
       <c r="O18" s="25"/>
       <c r="P18" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q18" s="8">
         <v>16</v>
@@ -2220,7 +2382,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B19" s="8">
         <v>4</v>
@@ -2238,7 +2400,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="26"/>
       <c r="H19" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I19" s="8">
         <v>4</v>
@@ -2267,7 +2429,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B20" s="8">
         <v>1</v>
@@ -2284,10 +2446,10 @@
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I20" s="8">
         <v>4</v>
@@ -2306,10 +2468,10 @@
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="P20" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Q20" s="8">
         <v>4</v>
@@ -2339,7 +2501,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="26"/>
       <c r="H21" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I21" s="8">
         <v>1</v>
@@ -2357,7 +2519,7 @@
       <c r="N21" s="3"/>
       <c r="O21" s="32"/>
       <c r="P21" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Q21" s="8">
         <v>4</v>
@@ -2399,7 +2561,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
@@ -2424,66 +2586,66 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I24" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="J24" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="K24" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J24" s="7" t="s">
+      <c r="L24" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="K24" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="L24" s="7" t="s">
-        <v>129</v>
       </c>
       <c r="M24" s="7"/>
       <c r="N24" s="3"/>
       <c r="O24" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P24" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="Q24" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="R24" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S24" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="T24" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="U24" s="36" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B25" s="8">
         <v>64</v>
@@ -2500,7 +2662,7 @@
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H25" s="7">
         <v>512</v>
@@ -2518,14 +2680,14 @@
         <v>768</v>
       </c>
       <c r="M25" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N25" s="3"/>
       <c r="O25" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="P25" s="35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="Q25" s="8">
         <v>64</v>
@@ -2547,7 +2709,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B26" s="8">
         <v>16</v>
@@ -2564,7 +2726,7 @@
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H26" s="7">
         <v>512</v>
@@ -2582,12 +2744,12 @@
         <v>1536</v>
       </c>
       <c r="M26" s="27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N26" s="3"/>
       <c r="O26" s="26"/>
       <c r="P26" s="34" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="Q26" s="8">
         <v>16</v>
@@ -2606,7 +2768,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B27" s="8">
         <v>4</v>
@@ -2623,7 +2785,7 @@
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H27" s="17">
         <v>1024</v>
@@ -2643,10 +2805,10 @@
       <c r="M27" s="29"/>
       <c r="N27" s="3"/>
       <c r="O27" s="30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="P27" s="34" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Q27" s="8">
         <v>16</v>
@@ -2668,7 +2830,7 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B28" s="8">
         <v>4</v>
@@ -2685,7 +2847,7 @@
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H28" s="7">
         <v>0</v>
@@ -2703,12 +2865,12 @@
         <v>512</v>
       </c>
       <c r="M28" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="N28" s="3"/>
       <c r="O28" s="31"/>
       <c r="P28" s="34" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Q28" s="8">
         <v>4</v>
@@ -2744,7 +2906,7 @@
       <c r="N29" s="3"/>
       <c r="O29" s="32"/>
       <c r="P29" s="34" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="Q29" s="8">
         <v>1</v>
@@ -2786,16 +2948,16 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E31" s="18"/>
       <c r="F31" s="3"/>
@@ -2817,7 +2979,7 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B32" s="19">
         <v>64</v>
@@ -2851,7 +3013,7 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="33" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B33" s="19">
         <v>16</v>
@@ -2885,7 +3047,7 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B34" s="19">
         <v>4</v>
@@ -2919,7 +3081,7 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B35" s="19">
         <v>1</v>
@@ -3000,11 +3162,13 @@
       <c r="U37" s="3"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="A38" s="44" t="s">
+        <v>204</v>
+      </c>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -3023,12 +3187,14 @@
       <c r="U38" s="3"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="A39" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="37"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -3046,12 +3212,23 @@
       <c r="U39" s="3"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="A40" s="42" t="s">
+        <v>211</v>
+      </c>
+      <c r="B40" s="43">
+        <v>128</v>
+      </c>
+      <c r="C40" s="47">
+        <v>1</v>
+      </c>
+      <c r="D40" s="38">
+        <v>4</v>
+      </c>
+      <c r="E40" s="38">
+        <f>B40*C40*D40</f>
+        <v>512</v>
+      </c>
+      <c r="F40" s="37"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
@@ -3069,12 +3246,23 @@
       <c r="U40" s="3"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="A41" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" s="38">
+        <v>256</v>
+      </c>
+      <c r="C41" s="38">
+        <v>1</v>
+      </c>
+      <c r="D41" s="38">
+        <v>4</v>
+      </c>
+      <c r="E41" s="38">
+        <f>B41*C41*D41</f>
+        <v>1024</v>
+      </c>
+      <c r="F41" s="37"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -3092,11 +3280,11 @@
       <c r="U41" s="3"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
+      <c r="A42" s="48"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -3115,12 +3303,14 @@
       <c r="U42" s="3"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="A43" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="37"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -3138,11 +3328,22 @@
       <c r="U43" s="3"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
+      <c r="A44" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="B44" s="40">
+        <v>64</v>
+      </c>
+      <c r="C44" s="40">
+        <v>4</v>
+      </c>
+      <c r="D44" s="41">
+        <v>4</v>
+      </c>
+      <c r="E44" s="41">
+        <f>B44*C44*D44</f>
+        <v>1024</v>
+      </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -3161,11 +3362,22 @@
       <c r="U44" s="3"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
+      <c r="A45" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="B45" s="8">
+        <v>32</v>
+      </c>
+      <c r="C45" s="7">
+        <v>4</v>
+      </c>
+      <c r="D45" s="7">
+        <v>2</v>
+      </c>
+      <c r="E45" s="7">
+        <f t="shared" ref="E45" si="7">B45*C45*D45</f>
+        <v>256</v>
+      </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -3184,11 +3396,11 @@
       <c r="U45" s="3"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
+      <c r="A46" s="45"/>
+      <c r="B46" s="45"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="45"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -3207,12 +3419,14 @@
       <c r="U46" s="3"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
+      <c r="A47" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="37"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -3230,12 +3444,23 @@
       <c r="U47" s="3"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
+      <c r="A48" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="B48" s="43">
+        <v>16</v>
+      </c>
+      <c r="C48" s="43">
+        <v>16</v>
+      </c>
+      <c r="D48" s="38">
+        <v>2</v>
+      </c>
+      <c r="E48" s="38">
+        <f t="shared" ref="E48:E50" si="8">B48*C48*D48</f>
+        <v>512</v>
+      </c>
+      <c r="F48" s="37"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
@@ -3253,11 +3478,22 @@
       <c r="U48" s="3"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
+      <c r="A49" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="B49" s="40">
+        <v>4</v>
+      </c>
+      <c r="C49" s="41">
+        <v>16</v>
+      </c>
+      <c r="D49" s="41">
+        <v>2</v>
+      </c>
+      <c r="E49" s="41">
+        <f t="shared" si="8"/>
+        <v>128</v>
+      </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
@@ -3276,11 +3512,22 @@
       <c r="U49" s="3"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
+      <c r="A50" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="B50" s="8">
+        <v>4</v>
+      </c>
+      <c r="C50" s="7">
+        <v>16</v>
+      </c>
+      <c r="D50" s="7">
+        <v>2</v>
+      </c>
+      <c r="E50" s="7">
+        <f t="shared" si="8"/>
+        <v>128</v>
+      </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -3299,11 +3546,11 @@
       <c r="U50" s="3"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -3322,11 +3569,13 @@
       <c r="U51" s="3"/>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
+      <c r="A52" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -3345,11 +3594,22 @@
       <c r="U52" s="3"/>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
+      <c r="A53" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="B53" s="8">
+        <v>4</v>
+      </c>
+      <c r="C53" s="8">
+        <v>72</v>
+      </c>
+      <c r="D53" s="7">
+        <v>2</v>
+      </c>
+      <c r="E53" s="7">
+        <f t="shared" ref="E53:E54" si="9">B53*C53*D53</f>
+        <v>576</v>
+      </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
@@ -3368,11 +3628,22 @@
       <c r="U53" s="3"/>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
+      <c r="A54" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="B54" s="8">
+        <v>4</v>
+      </c>
+      <c r="C54" s="8">
+        <v>72</v>
+      </c>
+      <c r="D54" s="7">
+        <v>2</v>
+      </c>
+      <c r="E54" s="7">
+        <f t="shared" si="9"/>
+        <v>576</v>
+      </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -3391,11 +3662,11 @@
       <c r="U54" s="3"/>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
@@ -6816,6 +7087,13 @@
       <c r="S203" s="3"/>
       <c r="T203" s="3"/>
       <c r="U203" s="3"/>
+    </row>
+    <row r="204" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A204" s="3"/>
+      <c r="B204" s="3"/>
+      <c r="C204" s="3"/>
+      <c r="D204" s="3"/>
+      <c r="E204" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -6854,7 +7132,7 @@
   <dimension ref="A1:AB19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6870,7 +7148,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H1" t="s">
         <v>17</v>
@@ -7262,7 +7540,7 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>195</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
@@ -7287,7 +7565,7 @@
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>196</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
@@ -7312,7 +7590,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
@@ -7337,7 +7615,7 @@
     </row>
     <row r="18" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
@@ -7393,7 +7671,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H1" t="s">
         <v>17</v>
@@ -9130,7 +9408,7 @@
   <dimension ref="A1:AB35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9145,7 +9423,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H1" t="s">
         <v>17</v>
@@ -9169,13 +9447,13 @@
         <v>24</v>
       </c>
       <c r="Q1" t="s">
+        <v>142</v>
+      </c>
+      <c r="R1" t="s">
+        <v>143</v>
+      </c>
+      <c r="S1" t="s">
         <v>144</v>
-      </c>
-      <c r="R1" t="s">
-        <v>145</v>
-      </c>
-      <c r="S1" t="s">
-        <v>146</v>
       </c>
       <c r="U1" t="s">
         <v>14</v>
@@ -9190,13 +9468,13 @@
         <v>24</v>
       </c>
       <c r="Z1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB1" t="s">
         <v>147</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>148</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
@@ -9288,7 +9566,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -9312,7 +9590,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B6">
         <f>B5+8</f>
@@ -9337,7 +9615,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B7">
         <f>B6+8</f>
@@ -9362,7 +9640,7 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B8">
         <f>B7+8</f>
@@ -9387,7 +9665,7 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C9">
         <f>E8</f>
@@ -9408,7 +9686,7 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C10">
         <f>F9</f>
@@ -9429,7 +9707,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C11">
         <f>F10</f>
@@ -9450,7 +9728,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B12">
         <f>D29-2</f>
@@ -9475,7 +9753,7 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C13">
         <f>E12</f>
@@ -9496,7 +9774,7 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C14">
         <f>F13</f>
@@ -9517,7 +9795,7 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C15">
         <f>F14</f>
@@ -9538,7 +9816,7 @@
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B16">
         <f>D32-2</f>
@@ -9563,7 +9841,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C17">
         <f>E16</f>
@@ -9584,7 +9862,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C18">
         <f>F17</f>
@@ -9605,7 +9883,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C19">
         <f>F18</f>
@@ -9626,7 +9904,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B20">
         <f>D35-2</f>
@@ -9651,7 +9929,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C21">
         <f>E20</f>
@@ -9672,7 +9950,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C22">
         <f>F21</f>
@@ -9693,7 +9971,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C23">
         <f>F22</f>
@@ -9731,7 +10009,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B25">
         <f>B8+8</f>
@@ -9756,7 +10034,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B26">
         <f>B25+8</f>
@@ -9781,7 +10059,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B27">
         <f>B26+8</f>
@@ -9806,7 +10084,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B28">
         <f>D27-2</f>
@@ -9831,7 +10109,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B29">
         <f>D28-2</f>
@@ -9856,7 +10134,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B30">
         <f>B12+8</f>
@@ -9881,7 +10159,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B31">
         <f>B30+8</f>
@@ -9906,7 +10184,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B32">
         <f>B31+8</f>
@@ -9931,7 +10209,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B33">
         <f>D16-2</f>
@@ -9956,7 +10234,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B34">
         <f>D33-2</f>
@@ -9981,7 +10259,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B35">
         <f>B34+8</f>
@@ -10012,10 +10290,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC0C317A-AECA-4343-96E0-4ED212B0C2E5}">
-  <dimension ref="A1:W18"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10031,7 +10309,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H1" t="s">
         <v>17</v>
@@ -10174,7 +10452,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -10210,10 +10488,10 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B6:B17" si="0">D5-2</f>
+        <f t="shared" ref="B6:B18" si="0">D5-2</f>
         <v>22</v>
       </c>
       <c r="C6">
@@ -10272,7 +10550,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
@@ -10297,7 +10575,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B9">
         <v>200</v>
@@ -10321,7 +10599,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
@@ -10396,7 +10674,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B13">
         <v>400</v>
@@ -10420,7 +10698,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
@@ -10445,85 +10723,110 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
+        <f>D14-2</f>
         <v>444</v>
       </c>
       <c r="C15">
-        <f>B15+$P$2</f>
+        <f>B15+$P$4</f>
         <v>446</v>
       </c>
       <c r="D15">
-        <f>C15+$Q$2</f>
-        <v>534</v>
+        <f>C15+$Q$4</f>
+        <v>490</v>
       </c>
       <c r="E15">
-        <f>D15+$R$2</f>
+        <f>D15+$R$4</f>
         <v>454</v>
       </c>
       <c r="F15">
-        <f>E15+$S$2</f>
-        <v>542</v>
+        <f>E15+$S$4</f>
+        <v>498</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B16">
+        <f>D15-2</f>
+        <v>488</v>
+      </c>
+      <c r="C16">
+        <f>B16+$P$4</f>
+        <v>490</v>
+      </c>
+      <c r="D16">
+        <f>C16+$Q$4</f>
+        <v>534</v>
+      </c>
+      <c r="E16">
+        <f>D16+$R$4</f>
+        <v>498</v>
+      </c>
+      <c r="F16">
+        <f>E16+$S$4</f>
+        <v>542</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>189</v>
+      </c>
+      <c r="B17">
         <v>600</v>
       </c>
-      <c r="C16">
-        <f>B16+$P$6</f>
+      <c r="C17">
+        <f>B17+$P$6</f>
         <v>602</v>
       </c>
-      <c r="D16">
-        <f>C16+$Q$6</f>
+      <c r="D17">
+        <f>C17+$Q$6</f>
         <v>624</v>
       </c>
-      <c r="E16">
-        <f>D16+$R$6</f>
+      <c r="E17">
+        <f>D17+$R$6</f>
         <v>610</v>
       </c>
-      <c r="F16">
-        <f>E16+$S$6</f>
+      <c r="F17">
+        <f>E17+$S$6</f>
         <v>631</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B17" s="1">
+    <row r="18" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B18" s="1">
         <f t="shared" si="0"/>
         <v>622</v>
       </c>
-      <c r="C17" s="1">
-        <f>B17+$P$4</f>
+      <c r="C18" s="1">
+        <f>B18+$P$4</f>
         <v>624</v>
       </c>
-      <c r="D17" s="1">
-        <f>C17+$Q$4</f>
+      <c r="D18" s="1">
+        <f>C18+$Q$4</f>
         <v>668</v>
       </c>
-      <c r="E17" s="1">
-        <f>D17+$R$4</f>
+      <c r="E18" s="1">
+        <f>D18+$R$4</f>
         <v>632</v>
       </c>
-      <c r="F17" s="1">
-        <f>E17+$S$4</f>
+      <c r="F18" s="1">
+        <f>E18+$S$4</f>
         <v>676</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -10537,7 +10840,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10553,40 +10856,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" t="s">
         <v>172</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>173</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>174</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>175</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>176</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>177</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>178</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>179</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>180</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>181</v>
-      </c>
-      <c r="K1" t="s">
-        <v>182</v>
-      </c>
-      <c r="L1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -11116,7 +11419,7 @@
       </c>
       <c r="G12" t="str">
         <f>'PMF c1 round0-3'!A15</f>
-        <v>PMF_M64_0</v>
+        <v>PMF_64M32_0</v>
       </c>
       <c r="H12">
         <f>'PMF c1 round0-3'!E15</f>
@@ -11128,7 +11431,7 @@
       </c>
       <c r="J12" t="str">
         <f>'PMF UV c1 round0-3'!A15</f>
-        <v>PMF_M32_a</v>
+        <v>PMF_32M16_0</v>
       </c>
       <c r="K12">
         <f>'PMF UV c1 round0-3'!E15</f>
@@ -11136,7 +11439,7 @@
       </c>
       <c r="L12">
         <f>'PMF UV c1 round0-3'!F15</f>
-        <v>542</v>
+        <v>498</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -11166,7 +11469,7 @@
       </c>
       <c r="G13" t="str">
         <f>'PMF c1 round0-3'!A16</f>
-        <v>PMF_M64_1</v>
+        <v>PMF_64M32_1</v>
       </c>
       <c r="H13">
         <f>'PMF c1 round0-3'!E16</f>
@@ -11177,15 +11480,15 @@
         <v>658</v>
       </c>
       <c r="J13" t="str">
-        <f>'PMF UV c1 round0-3'!A16</f>
+        <f>'PMF UV c1 round0-3'!A17</f>
         <v>PMF_F8_3</v>
       </c>
       <c r="K13">
-        <f>'PMF UV c1 round0-3'!E16</f>
+        <f>'PMF UV c1 round0-3'!E17</f>
         <v>610</v>
       </c>
       <c r="L13">
-        <f>'PMF UV c1 round0-3'!F16</f>
+        <f>'PMF UV c1 round0-3'!F17</f>
         <v>631</v>
       </c>
     </row>
@@ -11227,15 +11530,15 @@
         <v>638</v>
       </c>
       <c r="J14" t="str">
-        <f>'PMF UV c1 round0-3'!A17</f>
+        <f>'PMF UV c1 round0-3'!A18</f>
         <v>PMF_M8_3_c</v>
       </c>
       <c r="K14">
-        <f>'PMF UV c1 round0-3'!E17</f>
+        <f>'PMF UV c1 round0-3'!E18</f>
         <v>632</v>
       </c>
       <c r="L14">
-        <f>'PMF UV c1 round0-3'!F17</f>
+        <f>'PMF UV c1 round0-3'!F18</f>
         <v>676</v>
       </c>
     </row>
@@ -11277,15 +11580,15 @@
         <v>661</v>
       </c>
       <c r="J15">
-        <f>'PMF UV c1 round0-3'!A18</f>
+        <f>'PMF UV c1 round0-3'!A19</f>
         <v>0</v>
       </c>
       <c r="K15">
-        <f>'PMF UV c1 round0-3'!E18</f>
+        <f>'PMF UV c1 round0-3'!E19</f>
         <v>0</v>
       </c>
       <c r="L15">
-        <f>'PMF UV c1 round0-3'!F18</f>
+        <f>'PMF UV c1 round0-3'!F19</f>
         <v>0</v>
       </c>
     </row>
@@ -11327,15 +11630,15 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <f>'PMF UV c1 round0-3'!A19</f>
+        <f>'PMF UV c1 round0-3'!A20</f>
         <v>0</v>
       </c>
       <c r="K16">
-        <f>'PMF UV c1 round0-3'!E19</f>
+        <f>'PMF UV c1 round0-3'!E20</f>
         <v>0</v>
       </c>
       <c r="L16">
-        <f>'PMF UV c1 round0-3'!F19</f>
+        <f>'PMF UV c1 round0-3'!F20</f>
         <v>0</v>
       </c>
     </row>
@@ -11377,15 +11680,15 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <f>'PMF UV c1 round0-3'!A20</f>
+        <f>'PMF UV c1 round0-3'!A21</f>
         <v>0</v>
       </c>
       <c r="K17">
-        <f>'PMF UV c1 round0-3'!E20</f>
+        <f>'PMF UV c1 round0-3'!E21</f>
         <v>0</v>
       </c>
       <c r="L17">
-        <f>'PMF UV c1 round0-3'!F20</f>
+        <f>'PMF UV c1 round0-3'!F21</f>
         <v>0</v>
       </c>
     </row>
@@ -11427,15 +11730,15 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <f>'PMF UV c1 round0-3'!A21</f>
+        <f>'PMF UV c1 round0-3'!A22</f>
         <v>0</v>
       </c>
       <c r="K18">
-        <f>'PMF UV c1 round0-3'!E21</f>
+        <f>'PMF UV c1 round0-3'!E22</f>
         <v>0</v>
       </c>
       <c r="L18">
-        <f>'PMF UV c1 round0-3'!F21</f>
+        <f>'PMF UV c1 round0-3'!F22</f>
         <v>0</v>
       </c>
     </row>
@@ -11477,15 +11780,15 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <f>'PMF UV c1 round0-3'!A22</f>
+        <f>'PMF UV c1 round0-3'!A23</f>
         <v>0</v>
       </c>
       <c r="K19">
-        <f>'PMF UV c1 round0-3'!E22</f>
+        <f>'PMF UV c1 round0-3'!E23</f>
         <v>0</v>
       </c>
       <c r="L19">
-        <f>'PMF UV c1 round0-3'!F22</f>
+        <f>'PMF UV c1 round0-3'!F23</f>
         <v>0</v>
       </c>
     </row>
@@ -11527,15 +11830,15 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <f>'PMF UV c1 round0-3'!A23</f>
+        <f>'PMF UV c1 round0-3'!A24</f>
         <v>0</v>
       </c>
       <c r="K20">
-        <f>'PMF UV c1 round0-3'!E23</f>
+        <f>'PMF UV c1 round0-3'!E24</f>
         <v>0</v>
       </c>
       <c r="L20">
-        <f>'PMF UV c1 round0-3'!F23</f>
+        <f>'PMF UV c1 round0-3'!F24</f>
         <v>0</v>
       </c>
     </row>
@@ -11577,15 +11880,15 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <f>'PMF UV c1 round0-3'!A24</f>
+        <f>'PMF UV c1 round0-3'!A25</f>
         <v>0</v>
       </c>
       <c r="K21">
-        <f>'PMF UV c1 round0-3'!E24</f>
+        <f>'PMF UV c1 round0-3'!E25</f>
         <v>0</v>
       </c>
       <c r="L21">
-        <f>'PMF UV c1 round0-3'!F24</f>
+        <f>'PMF UV c1 round0-3'!F25</f>
         <v>0</v>
       </c>
     </row>
@@ -11627,15 +11930,15 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <f>'PMF UV c1 round0-3'!A25</f>
+        <f>'PMF UV c1 round0-3'!A26</f>
         <v>0</v>
       </c>
       <c r="K22">
-        <f>'PMF UV c1 round0-3'!E25</f>
+        <f>'PMF UV c1 round0-3'!E26</f>
         <v>0</v>
       </c>
       <c r="L22">
-        <f>'PMF UV c1 round0-3'!F25</f>
+        <f>'PMF UV c1 round0-3'!F26</f>
         <v>0</v>
       </c>
     </row>
@@ -11677,15 +11980,15 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <f>'PMF UV c1 round0-3'!A26</f>
+        <f>'PMF UV c1 round0-3'!A27</f>
         <v>0</v>
       </c>
       <c r="K23">
-        <f>'PMF UV c1 round0-3'!E26</f>
+        <f>'PMF UV c1 round0-3'!E27</f>
         <v>0</v>
       </c>
       <c r="L23">
-        <f>'PMF UV c1 round0-3'!F26</f>
+        <f>'PMF UV c1 round0-3'!F27</f>
         <v>0</v>
       </c>
     </row>
@@ -11727,15 +12030,15 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <f>'PMF UV c1 round0-3'!A27</f>
+        <f>'PMF UV c1 round0-3'!A28</f>
         <v>0</v>
       </c>
       <c r="K24">
-        <f>'PMF UV c1 round0-3'!E27</f>
+        <f>'PMF UV c1 round0-3'!E28</f>
         <v>0</v>
       </c>
       <c r="L24">
-        <f>'PMF UV c1 round0-3'!F27</f>
+        <f>'PMF UV c1 round0-3'!F28</f>
         <v>0</v>
       </c>
     </row>
@@ -11777,15 +12080,15 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <f>'PMF UV c1 round0-3'!A28</f>
+        <f>'PMF UV c1 round0-3'!A29</f>
         <v>0</v>
       </c>
       <c r="K25">
-        <f>'PMF UV c1 round0-3'!E28</f>
+        <f>'PMF UV c1 round0-3'!E29</f>
         <v>0</v>
       </c>
       <c r="L25">
-        <f>'PMF UV c1 round0-3'!F28</f>
+        <f>'PMF UV c1 round0-3'!F29</f>
         <v>0</v>
       </c>
     </row>
@@ -11827,15 +12130,15 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <f>'PMF UV c1 round0-3'!A29</f>
+        <f>'PMF UV c1 round0-3'!A30</f>
         <v>0</v>
       </c>
       <c r="K26">
-        <f>'PMF UV c1 round0-3'!E29</f>
+        <f>'PMF UV c1 round0-3'!E30</f>
         <v>0</v>
       </c>
       <c r="L26">
-        <f>'PMF UV c1 round0-3'!F29</f>
+        <f>'PMF UV c1 round0-3'!F30</f>
         <v>0</v>
       </c>
     </row>
@@ -11877,15 +12180,15 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <f>'PMF UV c1 round0-3'!A30</f>
+        <f>'PMF UV c1 round0-3'!A31</f>
         <v>0</v>
       </c>
       <c r="K27">
-        <f>'PMF UV c1 round0-3'!E30</f>
+        <f>'PMF UV c1 round0-3'!E31</f>
         <v>0</v>
       </c>
       <c r="L27">
-        <f>'PMF UV c1 round0-3'!F30</f>
+        <f>'PMF UV c1 round0-3'!F31</f>
         <v>0</v>
       </c>
     </row>
@@ -11927,15 +12230,15 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <f>'PMF UV c1 round0-3'!A31</f>
+        <f>'PMF UV c1 round0-3'!A32</f>
         <v>0</v>
       </c>
       <c r="K28">
-        <f>'PMF UV c1 round0-3'!E31</f>
+        <f>'PMF UV c1 round0-3'!E32</f>
         <v>0</v>
       </c>
       <c r="L28">
-        <f>'PMF UV c1 round0-3'!F31</f>
+        <f>'PMF UV c1 round0-3'!F32</f>
         <v>0</v>
       </c>
     </row>
@@ -11977,15 +12280,15 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <f>'PMF UV c1 round0-3'!A32</f>
+        <f>'PMF UV c1 round0-3'!A33</f>
         <v>0</v>
       </c>
       <c r="K29">
-        <f>'PMF UV c1 round0-3'!E32</f>
+        <f>'PMF UV c1 round0-3'!E33</f>
         <v>0</v>
       </c>
       <c r="L29">
-        <f>'PMF UV c1 round0-3'!F32</f>
+        <f>'PMF UV c1 round0-3'!F33</f>
         <v>0</v>
       </c>
     </row>
@@ -12027,15 +12330,15 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <f>'PMF UV c1 round0-3'!A33</f>
+        <f>'PMF UV c1 round0-3'!A34</f>
         <v>0</v>
       </c>
       <c r="K30">
-        <f>'PMF UV c1 round0-3'!E33</f>
+        <f>'PMF UV c1 round0-3'!E34</f>
         <v>0</v>
       </c>
       <c r="L30">
-        <f>'PMF UV c1 round0-3'!F33</f>
+        <f>'PMF UV c1 round0-3'!F34</f>
         <v>0</v>
       </c>
     </row>
@@ -12077,15 +12380,15 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <f>'PMF UV c1 round0-3'!A34</f>
+        <f>'PMF UV c1 round0-3'!A35</f>
         <v>0</v>
       </c>
       <c r="K31">
-        <f>'PMF UV c1 round0-3'!E34</f>
+        <f>'PMF UV c1 round0-3'!E35</f>
         <v>0</v>
       </c>
       <c r="L31">
-        <f>'PMF UV c1 round0-3'!F34</f>
+        <f>'PMF UV c1 round0-3'!F35</f>
         <v>0</v>
       </c>
     </row>
@@ -12127,15 +12430,15 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <f>'PMF UV c1 round0-3'!A35</f>
+        <f>'PMF UV c1 round0-3'!A36</f>
         <v>0</v>
       </c>
       <c r="K32">
-        <f>'PMF UV c1 round0-3'!E35</f>
+        <f>'PMF UV c1 round0-3'!E36</f>
         <v>0</v>
       </c>
       <c r="L32">
-        <f>'PMF UV c1 round0-3'!F35</f>
+        <f>'PMF UV c1 round0-3'!F36</f>
         <v>0</v>
       </c>
     </row>
@@ -12177,15 +12480,15 @@
         <v>0</v>
       </c>
       <c r="J33">
-        <f>'PMF UV c1 round0-3'!A36</f>
+        <f>'PMF UV c1 round0-3'!A37</f>
         <v>0</v>
       </c>
       <c r="K33">
-        <f>'PMF UV c1 round0-3'!E36</f>
+        <f>'PMF UV c1 round0-3'!E37</f>
         <v>0</v>
       </c>
       <c r="L33">
-        <f>'PMF UV c1 round0-3'!F36</f>
+        <f>'PMF UV c1 round0-3'!F37</f>
         <v>0</v>
       </c>
     </row>
@@ -12227,15 +12530,15 @@
         <v>0</v>
       </c>
       <c r="J34">
-        <f>'PMF UV c1 round0-3'!A37</f>
+        <f>'PMF UV c1 round0-3'!A38</f>
         <v>0</v>
       </c>
       <c r="K34">
-        <f>'PMF UV c1 round0-3'!E37</f>
+        <f>'PMF UV c1 round0-3'!E38</f>
         <v>0</v>
       </c>
       <c r="L34">
-        <f>'PMF UV c1 round0-3'!F37</f>
+        <f>'PMF UV c1 round0-3'!F38</f>
         <v>0</v>
       </c>
     </row>
@@ -12277,15 +12580,15 @@
         <v>0</v>
       </c>
       <c r="J35">
-        <f>'PMF UV c1 round0-3'!A38</f>
+        <f>'PMF UV c1 round0-3'!A39</f>
         <v>0</v>
       </c>
       <c r="K35">
-        <f>'PMF UV c1 round0-3'!E38</f>
+        <f>'PMF UV c1 round0-3'!E39</f>
         <v>0</v>
       </c>
       <c r="L35">
-        <f>'PMF UV c1 round0-3'!F38</f>
+        <f>'PMF UV c1 round0-3'!F39</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>